<commit_message>
change in projects file
</commit_message>
<xml_diff>
--- a/Projects.xlsx
+++ b/Projects.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>S.No.</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>karthickseetha2@gmail.com</t>
+  </si>
+  <si>
+    <t>Arun Kumar</t>
+  </si>
+  <si>
+    <t>arunabi1819@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -322,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +391,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,7 +679,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,9 +1078,15 @@
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="3"/>
+      <c r="B17" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="3">
+        <v>6374247005</v>
+      </c>
       <c r="E17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1333,8 +1348,9 @@
     <hyperlink ref="C15" r:id="rId38"/>
     <hyperlink ref="C16" r:id="rId39"/>
     <hyperlink ref="C21" r:id="rId40"/>
+    <hyperlink ref="C17" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>